<commit_message>
Add linear gradient measurement
</commit_message>
<xml_diff>
--- a/spindleSpeeds.xlsx
+++ b/spindleSpeeds.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t xml:space="preserve">commanded</t>
   </si>
@@ -67,13 +68,23 @@
   <si>
     <t xml:space="preserve">New scale</t>
   </si>
+  <si>
+    <t xml:space="preserve">Scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Actual – com abs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% Actual – com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -151,8 +162,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -228,7 +243,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -276,57 +291,72 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$9:$B$21</c:f>
+              <c:f>Sheet2!$A$9:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>250</c:v>
+                  <c:v>266</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>500</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>600</c:v>
+                  <c:v>612</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>750</c:v>
+                  <c:v>760</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1250</c:v>
+                  <c:v>1243</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1500</c:v>
+                  <c:v>1480</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2000</c:v>
+                  <c:v>1720</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2500</c:v>
+                  <c:v>1953</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3000</c:v>
+                  <c:v>2188</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3500</c:v>
+                  <c:v>2413</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4000</c:v>
+                  <c:v>2870</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4500</c:v>
+                  <c:v>3350</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3821</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4202</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4762</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5241</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5717</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$9:$D$21</c:f>
+              <c:f>Sheet2!$D$9:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>26.8528464017186</c:v>
                 </c:pt>
@@ -343,28 +373,43 @@
                   <c:v>28.5714285714286</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28.8018433179723</c:v>
+                  <c:v>28.8018433179724</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>28.957528957529</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>29.0697674418605</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>33.2225913621262</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>29.381039435884</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>36.4431486880466</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>38.961038961039</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>40.983606557377</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>29.9177262528048</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>30.6122448979592</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30.0120048019208</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29.9890948745911</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -410,57 +455,72 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$9:$B$21</c:f>
+              <c:f>Sheet2!$A$9:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>250</c:v>
+                  <c:v>266</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>500</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>600</c:v>
+                  <c:v>612</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>750</c:v>
+                  <c:v>760</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1250</c:v>
+                  <c:v>1243</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1500</c:v>
+                  <c:v>1480</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2000</c:v>
+                  <c:v>1720</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2500</c:v>
+                  <c:v>1953</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3000</c:v>
+                  <c:v>2188</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3500</c:v>
+                  <c:v>2413</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4000</c:v>
+                  <c:v>2870</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4500</c:v>
+                  <c:v>3350</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3821</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4202</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4762</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5241</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5717</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$E$9:$E$21</c:f>
+              <c:f>Sheet2!$E$9:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>28.5714285714286</c:v>
                 </c:pt>
@@ -483,22 +543,37 @@
                   <c:v>28.5714285714286</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>28.5714285714286</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>32.4418604651163</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
+                  <c:v>28.5714285714286</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>35.1749271137026</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>37.2727272727273</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>39.2271662763466</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>28.5789080029918</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>28.5850340136054</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28.5834333733493</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28.576881134133</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28.585</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -513,11 +588,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="48541531"/>
-        <c:axId val="82499007"/>
+        <c:axId val="50004353"/>
+        <c:axId val="65185337"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48541531"/>
+        <c:axId val="50004353"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -552,14 +627,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82499007"/>
+        <c:crossAx val="65185337"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82499007"/>
+        <c:axId val="65185337"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -603,7 +678,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48541531"/>
+        <c:crossAx val="50004353"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -640,7 +715,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -684,6 +759,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -707,10 +783,10 @@
           </c:trendline>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$F$10:$F$19</c:f>
+              <c:f>Sheet2!$F$10:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.68886337543054</c:v>
                 </c:pt>
@@ -724,22 +800,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.161290322580644</c:v>
+                  <c:v>-0.161290322580648</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-0.386100386100384</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>-0.498338870431894</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>-0.780730897009967</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>-1.26822157434402</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.68831168831169</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1.75644028103044</c:v>
+                  <c:v>-0.809610864455472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -754,11 +827,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="86299949"/>
-        <c:axId val="35734457"/>
+        <c:axId val="91710277"/>
+        <c:axId val="7201187"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86299949"/>
+        <c:axId val="91710277"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -793,14 +866,336 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35734457"/>
+        <c:crossAx val="7201187"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35734457"/>
+        <c:axId val="7201187"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="91710277"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="004586"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="0"/>
+            <c:backward val="0"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$4:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$4:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1445</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1744</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2359</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2669</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2982</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3580</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5990</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="79490528"/>
+        <c:axId val="61659886"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="79490528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="61659886"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="61659886"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -844,7 +1239,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86299949"/>
+        <c:crossAx val="79490528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -858,14 +1253,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="-6.25039064941559E-005"/>
-          <c:y val="0"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -874,7 +1263,7 @@
       </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="span"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -892,9 +1281,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>713880</xdr:colOff>
+      <xdr:colOff>714240</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
@@ -908,8 +1297,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5590440" y="162720"/>
-        <a:ext cx="5798520" cy="1896840"/>
+        <a:off x="5590800" y="163080"/>
+        <a:ext cx="5798160" cy="1896480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -921,16 +1310,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>565200</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>436680</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>634320</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>506160</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>47880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -938,12 +1327,47 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5441760" y="2323440"/>
-        <a:ext cx="5758920" cy="3241800"/>
+        <a:off x="6126120" y="2333880"/>
+        <a:ext cx="5758920" cy="4053600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>497520</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>143640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>560520</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>134280</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="5901120" y="956160"/>
+        <a:ext cx="5752800" cy="3241800"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1211,10 +1635,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1438,7 +1862,7 @@
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">B14/C14</f>
-        <v>28.8018433179723</v>
+        <v>28.8018433179724</v>
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">A14/C14</f>
@@ -1446,7 +1870,7 @@
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">E14-D14</f>
-        <v>-0.161290322580644</v>
+        <v>-0.161290322580648</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">C14/A14</f>
@@ -1482,197 +1906,332 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>1953</v>
+        <v>1720</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>2000</v>
+        <v>1750</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>60.2</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">B16/C16</f>
-        <v>33.2225913621262</v>
+        <v>29.0697674418605</v>
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">A16/C16</f>
-        <v>32.4418604651163</v>
+        <v>28.5714285714286</v>
       </c>
       <c r="F16" s="0" t="n">
         <f aca="false">E16-D16</f>
-        <v>-0.780730897009967</v>
+        <v>-0.498338870431894</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">C16/A16</f>
-        <v>0.0308243727598566</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>2413</v>
+        <v>1953</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>68.6</v>
+        <v>60.2</v>
       </c>
       <c r="D17" s="0" t="n">
         <f aca="false">B17/C17</f>
-        <v>36.4431486880466</v>
+        <v>33.2225913621262</v>
       </c>
       <c r="E17" s="0" t="n">
         <f aca="false">A17/C17</f>
-        <v>35.1749271137026</v>
+        <v>32.4418604651163</v>
       </c>
       <c r="F17" s="0" t="n">
         <f aca="false">E17-D17</f>
-        <v>-1.26822157434402</v>
+        <v>-0.780730897009967</v>
       </c>
       <c r="G17" s="0" t="n">
         <f aca="false">C17/A17</f>
-        <v>0.0284293410692085</v>
+        <v>0.0308243727598566</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>2870</v>
+        <v>2188</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>3000</v>
+        <v>2250</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>77</v>
+        <v>76.58</v>
       </c>
       <c r="D18" s="0" t="n">
         <f aca="false">B18/C18</f>
-        <v>38.961038961039</v>
+        <v>29.381039435884</v>
       </c>
       <c r="E18" s="0" t="n">
         <f aca="false">A18/C18</f>
-        <v>37.2727272727273</v>
+        <v>28.5714285714286</v>
       </c>
       <c r="F18" s="0" t="n">
         <f aca="false">E18-D18</f>
-        <v>-1.68831168831169</v>
+        <v>-0.809610864455472</v>
       </c>
       <c r="G18" s="0" t="n">
         <f aca="false">C18/A18</f>
-        <v>0.0268292682926829</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>3350</v>
+        <v>2413</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>3500</v>
+        <v>2500</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>85.4</v>
+        <v>68.6</v>
       </c>
       <c r="D19" s="0" t="n">
         <f aca="false">B19/C19</f>
-        <v>40.983606557377</v>
+        <v>36.4431486880466</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">A19/C19</f>
-        <v>39.2271662763466</v>
+        <v>35.1749271137026</v>
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">E19-D19</f>
-        <v>-1.75644028103044</v>
+        <v>-1.26822157434402</v>
       </c>
       <c r="G19" s="0" t="n">
         <f aca="false">C19/A19</f>
-        <v>0.0254925373134328</v>
+        <v>0.0284293410692085</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>3821</v>
+        <v>2870</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>133.7</v>
+        <v>77</v>
       </c>
       <c r="D20" s="0" t="n">
         <f aca="false">B20/C20</f>
-        <v>29.9177262528048</v>
+        <v>38.961038961039</v>
       </c>
       <c r="E20" s="0" t="n">
         <f aca="false">A20/C20</f>
-        <v>28.5789080029918</v>
+        <v>37.2727272727273</v>
       </c>
       <c r="F20" s="0" t="n">
         <f aca="false">E20-D20</f>
-        <v>-1.33881824981302</v>
+        <v>-1.68831168831169</v>
       </c>
       <c r="G20" s="0" t="n">
         <f aca="false">C20/A20</f>
-        <v>0.0349908400942162</v>
+        <v>0.0268292682926829</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>4202</v>
+        <v>3350</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>4500</v>
+        <v>3500</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>147</v>
+        <v>85.4</v>
       </c>
       <c r="D21" s="0" t="n">
         <f aca="false">B21/C21</f>
-        <v>30.6122448979592</v>
+        <v>40.983606557377</v>
       </c>
       <c r="E21" s="0" t="n">
         <f aca="false">A21/C21</f>
-        <v>28.5850340136054</v>
+        <v>39.2271662763466</v>
       </c>
       <c r="F21" s="0" t="n">
         <f aca="false">E21-D21</f>
-        <v>-2.02721088435374</v>
+        <v>-1.75644028103044</v>
       </c>
       <c r="G21" s="0" t="n">
         <f aca="false">C21/A21</f>
+        <v>0.0254925373134328</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>3821</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>133.7</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">B22/C22</f>
+        <v>29.9177262528048</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <f aca="false">A22/C22</f>
+        <v>28.5789080029918</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <f aca="false">E22-D22</f>
+        <v>-1.33881824981302</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <f aca="false">C22/A22</f>
+        <v>0.0349908400942162</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>4202</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>4500</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">B23/C23</f>
+        <v>30.6122448979592</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <f aca="false">A23/C23</f>
+        <v>28.5850340136054</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <f aca="false">E23-D23</f>
+        <v>-2.02721088435374</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <f aca="false">C23/A23</f>
         <v>0.0349833412660638</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>4762</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>166.6</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">B24/C24</f>
+        <v>30.0120048019208</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <f aca="false">A24/C24</f>
+        <v>28.5834333733493</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <f aca="false">E24-D24</f>
+        <v>-1.42857142857143</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <f aca="false">C24/A24</f>
+        <v>0.0349853002939941</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>5241</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>5500</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>183.4</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <f aca="false">B25/C25</f>
+        <v>29.9890948745911</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <f aca="false">A25/C25</f>
+        <v>28.576881134133</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <f aca="false">E25-D25</f>
+        <v>-1.41221374045801</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <f aca="false">C25/A25</f>
+        <v>0.0349933218851364</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>5717</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>6000</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <f aca="false">B26/C26</f>
+        <v>30</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <f aca="false">A26/C26</f>
+        <v>28.585</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <f aca="false">E26-D26</f>
+        <v>-1.415</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">C26/A26</f>
+        <v>0.0349833828931258</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="0" t="n">
-        <v>0.976787973</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="B27" s="0" t="n">
+        <v>0.98258155</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="0" t="n">
-        <f aca="false">1/B22</f>
-        <v>1.02376362899792</v>
-      </c>
-      <c r="D23" s="0" t="s">
+      <c r="B28" s="0" t="n">
+        <f aca="false">1/B27</f>
+        <v>1.01772723088481</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="0" t="n">
-        <f aca="false">AVERAGE(G9:G21)</f>
-        <v>0.0327298973266451</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="E28" s="0" t="n">
+        <f aca="false">AVERAGE(G9:G23)</f>
+        <v>0.0330325776830924</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="0" t="n">
-        <f aca="false">B7*B23</f>
-        <v>0.0358317270149271</v>
+      <c r="B29" s="0" t="n">
+        <f aca="false">B7*B28</f>
+        <v>0.0356204530809682</v>
       </c>
     </row>
   </sheetData>
@@ -1685,4 +2244,350 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M42"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">B4-I33</f>
+        <v>170</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <f aca="false">D4/B4</f>
+        <v>0.62962962962963</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>560</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">B5-I34</f>
+        <v>360</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <f aca="false">D5/B5</f>
+        <v>0.642857142857143</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1445</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">B8-I35</f>
+        <v>945</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <f aca="false">D8/B8</f>
+        <v>0.653979238754325</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1744</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">B9-I36</f>
+        <v>1144</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <f aca="false">D9/B9</f>
+        <v>0.655963302752294</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>2359</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">B11-I38</f>
+        <v>1559</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <f aca="false">D11/B11</f>
+        <v>0.660873251377702</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>2669</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">B12-I39</f>
+        <v>1769</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <f aca="false">D12/B12</f>
+        <v>0.662795054327463</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>2982</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">B13-I40</f>
+        <v>1982</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <f aca="false">D13/B13</f>
+        <v>0.664654594232059</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>1200</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>3580</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">B15-I41</f>
+        <v>2380</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <f aca="false">D15/B15</f>
+        <v>0.664804469273743</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>5990</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">B23-I42</f>
+        <v>3990</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <f aca="false">D23/B23</f>
+        <v>0.666110183639399</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I33" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I34" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I35" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I36" s="0" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I37" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>2203</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="L37" s="0" t="n">
+        <f aca="false">J37-I37</f>
+        <v>1453</v>
+      </c>
+      <c r="M37" s="1" t="n">
+        <f aca="false">L37/J37</f>
+        <v>0.659555152065365</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I38" s="0" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I39" s="0" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I40" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I41" s="0" t="n">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I42" s="0" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Near perfect spindle scaling
Thanks, spreadsheets
</commit_message>
<xml_diff>
--- a/spindleSpeeds.xlsx
+++ b/spindleSpeeds.xlsx
@@ -5,12 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
   <si>
     <t xml:space="preserve">commanded</t>
   </si>
@@ -77,6 +80,30 @@
   <si>
     <t xml:space="preserve">% Actual – com</t>
   </si>
+  <si>
+    <t xml:space="preserve">Slope:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPM offset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offset:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average difference:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New scale:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offset dleta:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New offset:</t>
+  </si>
 </sst>
 </file>
 
@@ -86,12 +113,11 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -111,11 +137,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -162,12 +183,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -243,7 +268,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -588,11 +613,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="73446689"/>
-        <c:axId val="89059120"/>
+        <c:axId val="18138918"/>
+        <c:axId val="47077141"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73446689"/>
+        <c:axId val="18138918"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -627,14 +652,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89059120"/>
+        <c:crossAx val="47077141"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89059120"/>
+        <c:axId val="47077141"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +703,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73446689"/>
+        <c:crossAx val="18138918"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -715,7 +740,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -827,11 +852,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="26561983"/>
-        <c:axId val="68975742"/>
+        <c:axId val="51672005"/>
+        <c:axId val="35774843"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="26561983"/>
+        <c:axId val="51672005"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,14 +891,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68975742"/>
+        <c:crossAx val="35774843"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68975742"/>
+        <c:axId val="35774843"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -917,7 +942,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26561983"/>
+        <c:crossAx val="51672005"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -954,7 +979,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1149,11 +1174,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="25369140"/>
-        <c:axId val="98047746"/>
+        <c:axId val="84128432"/>
+        <c:axId val="3880429"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="25369140"/>
+        <c:axId val="84128432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1188,14 +1213,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98047746"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="3880429"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98047746"/>
+        <c:axId val="3880429"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,7 +1264,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25369140"/>
+        <c:crossAx val="84128432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1281,15 +1306,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>714240</xdr:colOff>
+      <xdr:colOff>714960</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>10080</xdr:colOff>
+      <xdr:colOff>10440</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1297,8 +1322,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5590800" y="163080"/>
-        <a:ext cx="5798160" cy="1896480"/>
+        <a:off x="5591520" y="163800"/>
+        <a:ext cx="5797800" cy="1896120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1313,13 +1338,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>436680</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>58320</xdr:rowOff>
+      <xdr:rowOff>59040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>506160</xdr:colOff>
+      <xdr:colOff>506520</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:rowOff>48240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1327,8 +1352,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6126120" y="2333880"/>
-        <a:ext cx="5758920" cy="4053600"/>
+        <a:off x="6126120" y="2334600"/>
+        <a:ext cx="5759280" cy="4053240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2253,8 +2278,8 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2300,13 +2325,13 @@
       <c r="C4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">B4-I33</f>
-        <v>170</v>
-      </c>
-      <c r="E4" s="1" t="n">
+      <c r="D4" s="0" t="e">
+        <f aca="false">B4-#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E4" s="1" t="e">
         <f aca="false">D4/B4</f>
-        <v>0.62962962962963</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2320,7 +2345,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="0" t="n">
-        <f aca="false">B5-I34</f>
+        <f aca="false">B5-I32</f>
         <v>360</v>
       </c>
       <c r="E5" s="1" t="n">
@@ -2349,7 +2374,7 @@
         <v>50</v>
       </c>
       <c r="D8" s="0" t="n">
-        <f aca="false">B8-I35</f>
+        <f aca="false">B8-I33</f>
         <v>945</v>
       </c>
       <c r="E8" s="1" t="n">
@@ -2367,13 +2392,13 @@
       <c r="C9" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="D9" s="0" t="n">
-        <f aca="false">B9-I36</f>
-        <v>1144</v>
-      </c>
-      <c r="E9" s="1" t="n">
+      <c r="D9" s="0" t="e">
+        <f aca="false">B9-#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E9" s="1" t="e">
         <f aca="false">D9/B9</f>
-        <v>0.655963302752294</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2392,7 +2417,7 @@
         <v>80</v>
       </c>
       <c r="D11" s="0" t="n">
-        <f aca="false">B11-I38</f>
+        <f aca="false">B11-I35</f>
         <v>1559</v>
       </c>
       <c r="E11" s="1" t="n">
@@ -2411,7 +2436,7 @@
         <v>90</v>
       </c>
       <c r="D12" s="0" t="n">
-        <f aca="false">B12-I39</f>
+        <f aca="false">B12-I36</f>
         <v>1769</v>
       </c>
       <c r="E12" s="1" t="n">
@@ -2429,13 +2454,13 @@
       <c r="C13" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="D13" s="0" t="n">
-        <f aca="false">B13-I40</f>
-        <v>1982</v>
-      </c>
-      <c r="E13" s="1" t="n">
+      <c r="D13" s="0" t="e">
+        <f aca="false">B13-#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E13" s="1" t="e">
         <f aca="false">D13/B13</f>
-        <v>0.664654594232059</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2454,7 +2479,7 @@
         <v>120</v>
       </c>
       <c r="D15" s="0" t="n">
-        <f aca="false">B15-I41</f>
+        <f aca="false">B15-I37</f>
         <v>2380</v>
       </c>
       <c r="E15" s="1" t="n">
@@ -2507,93 +2532,909 @@
       <c r="C23" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="D23" s="0" t="n">
-        <f aca="false">B23-I42</f>
-        <v>3990</v>
-      </c>
-      <c r="E23" s="1" t="n">
+      <c r="D23" s="0" t="e">
+        <f aca="false">B23-#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E23" s="1" t="e">
         <f aca="false">D23/B23</f>
-        <v>0.666110183639399</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="e">
-        <f aca="false">LINEST(A4:A23,B4:B23,1,1)</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <f aca="false">B30-I48</f>
+        <v>270</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <f aca="false">D30/B30</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>560</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <f aca="false">B31-I49</f>
+        <v>560</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <f aca="false">D31/B31</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1445</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <f aca="false">B32-I50</f>
+        <v>1445</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <f aca="false">D32/B32</f>
+        <v>1</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>1744</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <f aca="false">B33-I51</f>
+        <v>1744</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <f aca="false">D33/B33</f>
+        <v>1</v>
+      </c>
       <c r="I33" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>2359</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <f aca="false">B34-I53</f>
+        <v>2359</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <f aca="false">D34/B34</f>
+        <v>1</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>2203</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="L34" s="0" t="n">
+        <f aca="false">J34-I34</f>
+        <v>1453</v>
+      </c>
+      <c r="M34" s="1" t="n">
+        <f aca="false">L34/J34</f>
+        <v>0.659555152065365</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>2669</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <f aca="false">B35-I54</f>
+        <v>2669</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <f aca="false">D35/B35</f>
+        <v>1</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>2982</v>
+      </c>
+      <c r="C36" s="0" t="n">
         <v>100</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I34" s="0" t="n">
+      <c r="D36" s="0" t="n">
+        <f aca="false">B36-I55</f>
+        <v>2982</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <f aca="false">D36/B36</f>
+        <v>1</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>1200</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>3580</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <f aca="false">B37-I56</f>
+        <v>3580</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <f aca="false">D37/B37</f>
+        <v>1</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>5990</v>
+      </c>
+      <c r="C38" s="0" t="n">
         <v>200</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I35" s="0" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I36" s="0" t="n">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I37" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="J37" s="0" t="n">
-        <v>2203</v>
-      </c>
-      <c r="K37" s="0" t="n">
-        <v>75</v>
-      </c>
-      <c r="L37" s="0" t="n">
-        <f aca="false">J37-I37</f>
-        <v>1453</v>
-      </c>
-      <c r="M37" s="1" t="n">
-        <f aca="false">L37/J37</f>
-        <v>0.659555152065365</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I38" s="0" t="n">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I39" s="0" t="n">
-        <v>900</v>
+      <c r="D38" s="0" t="n">
+        <f aca="false">B38-I57</f>
+        <v>5990</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <f aca="false">D38/B38</f>
+        <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I40" s="0" t="n">
-        <v>1000</v>
+      <c r="A40" s="0" t="n">
+        <f aca="false">B1*LINEST(A30:A38,B30:B38,1,1)</f>
+        <v>0.03312450571748</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <f aca="false">B1*SLOPE(A30:A38,B30:B38)</f>
+        <v>0.03312450571748</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I41" s="0" t="n">
-        <v>1200</v>
+      <c r="A41" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I42" s="0" t="n">
-        <v>2000</v>
+      <c r="A42" s="0" t="n">
+        <f aca="false">Sheet4!E13*Sheet4!B15</f>
+        <v>1.51174264312703</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>0.03312450571748</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>3.31</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">A4-B4</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>172</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>6.62</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">A5-B5</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>16.56</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">A6-B6</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>943</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>33.12</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">A7-B7</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1432</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>49.68</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">A8-B8</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1936</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>66.24</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">A9-B9</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>6000</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>5950</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>198.7</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">A10-B10</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>2960</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>99.37</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">A11-B11</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">SLOPE(A4:A11,B4:B11)</f>
+        <v>1.00303724738225</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <f aca="false">AVERAGE(D4:D11)</f>
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">B1*B13</f>
+        <v>0.0332251130357588</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <f aca="false">E13*B15</f>
+        <v>1.51174264312703</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>0.033225113035759</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1.51174264312703</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>505</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>18.12</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">A4-B4</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>991</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>34.73</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">A5-B5</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1480</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>51.34</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">A6-B6</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1985</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>67.96</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">A7-B7</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>2500</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2496</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>84.57</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">A8-B8</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>3020</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>101.1</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">A9-B9</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>4020</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>134.4</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">A10-B10</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>5020</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>167.6</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">A11-B11</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>6000</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>6020</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>200.8</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">A12-B12</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">SLOPE(A4:A12,B4:B12)</f>
+        <v>0.993508089795602</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">AVERAGE(D4:D12)</f>
+        <v>-4.11111111111111</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <f aca="false">B1*1/B14</f>
+        <v>0.0334422169049419</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <f aca="false">E14*B16</f>
+        <v>-0.137484669498094</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <f aca="false">B2+B18</f>
+        <v>1.37425797362894</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <f aca="false">Sheet5!B1</f>
+        <v>0.033225113035759</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">Sheet5!B2</f>
+        <v>1.51174264312703</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>505</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">A4-B4</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>994</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">A5-B5</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1491</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">A6-B6</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1995</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">A7-B7</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>2500</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2510</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">A8-B8</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>3034</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">A9-B9</f>
+        <v>-34</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>4043</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">A10-B10</f>
+        <v>-43</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>5055</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">A11-B11</f>
+        <v>-55</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>6000</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>6055</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">A12-B12</f>
+        <v>-55</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">SLOPE(A4:A12,B4:B12)</f>
+        <v>0.98699975620218</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">AVERAGE(D4:D12)</f>
+        <v>-20.2222222222222</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <f aca="false">B1*1/B14</f>
+        <v>0.0336627368213382</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <f aca="false">E14*B16</f>
+        <v>-0.680735344609284</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <f aca="false">B2+B18</f>
+        <v>0.831007298517746</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>